<commit_message>
Fixed audio panning and videoSegmentData.csv for up to 040. Added missing images that I forgot to commit earlier.
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A11_photos.xlsx
+++ b/MISSION_DATA/A11_photos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="465" windowWidth="38400" windowHeight="22515"/>
+    <workbookView xWindow="8145" yWindow="465" windowWidth="38400" windowHeight="22515"/>
   </bookViews>
   <sheets>
     <sheet name="A11_photos" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="5002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="5005">
   <si>
     <t>S69-31741</t>
   </si>
@@ -15029,6 +15029,15 @@
   </si>
   <si>
     <t>086:29:16</t>
+  </si>
+  <si>
+    <t>003:23:16</t>
+  </si>
+  <si>
+    <t>003:23:26</t>
+  </si>
+  <si>
+    <t>003:23:31</t>
   </si>
 </sst>
 </file>
@@ -15846,8 +15855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17250,7 +17259,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>2575</v>
+        <v>5002</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>1176</v>
@@ -17264,7 +17273,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>4992</v>
+        <v>5003</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>1178</v>
@@ -17278,7 +17287,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>4993</v>
+        <v>5004</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>1180</v>

</xml_diff>

<commit_message>
Fixed audio panning and videoSegmentData.csv for up to 120.
</commit_message>
<xml_diff>
--- a/MISSION_DATA/A11_photos.xlsx
+++ b/MISSION_DATA/A11_photos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8145" yWindow="465" windowWidth="38400" windowHeight="22515"/>
+    <workbookView xWindow="8145" yWindow="465" windowWidth="11970" windowHeight="11925"/>
   </bookViews>
   <sheets>
     <sheet name="A11_photos" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="5005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7384" uniqueCount="5006">
   <si>
     <t>S69-31741</t>
   </si>
@@ -13975,12 +13975,6 @@
     <t>009:54:00</t>
   </si>
   <si>
-    <t>011:47:08</t>
-  </si>
-  <si>
-    <t>011:47:17</t>
-  </si>
-  <si>
     <t>011:47:25</t>
   </si>
   <si>
@@ -15038,6 +15032,15 @@
   </si>
   <si>
     <t>003:23:31</t>
+  </si>
+  <si>
+    <t>010:35:26</t>
+  </si>
+  <si>
+    <t>010:35:31</t>
+  </si>
+  <si>
+    <t>010:35:36</t>
   </si>
 </sst>
 </file>
@@ -15855,8 +15858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1317"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15933,7 +15936,7 @@
         <v>3561</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>4673</v>
+        <v>4671</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -17217,7 +17220,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
-        <v>4992</v>
+        <v>4990</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>1170</v>
@@ -17231,7 +17234,7 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
-        <v>4993</v>
+        <v>4991</v>
       </c>
       <c r="B118" s="4" t="s">
         <v>1172</v>
@@ -17245,7 +17248,7 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
-        <v>4994</v>
+        <v>4992</v>
       </c>
       <c r="B119" s="4" t="s">
         <v>1174</v>
@@ -17259,7 +17262,7 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
-        <v>5002</v>
+        <v>5000</v>
       </c>
       <c r="B120" s="4" t="s">
         <v>1176</v>
@@ -17273,7 +17276,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
-        <v>5003</v>
+        <v>5001</v>
       </c>
       <c r="B121" s="4" t="s">
         <v>1178</v>
@@ -17287,7 +17290,7 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
-        <v>5004</v>
+        <v>5002</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>1180</v>
@@ -17637,7 +17640,7 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
-        <v>4378</v>
+        <v>5003</v>
       </c>
       <c r="B147" s="4" t="s">
         <v>1134</v>
@@ -17651,7 +17654,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
-        <v>4650</v>
+        <v>5004</v>
       </c>
       <c r="B148" s="4" t="s">
         <v>1133</v>
@@ -17665,7 +17668,7 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
-        <v>4651</v>
+        <v>5005</v>
       </c>
       <c r="B149" s="4" t="s">
         <v>1135</v>
@@ -17679,7 +17682,7 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
-        <v>4652</v>
+        <v>4650</v>
       </c>
       <c r="B150" s="4" t="s">
         <v>1137</v>
@@ -17693,7 +17696,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
-        <v>4653</v>
+        <v>4651</v>
       </c>
       <c r="B151" s="4" t="s">
         <v>1139</v>
@@ -17707,7 +17710,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
-        <v>4654</v>
+        <v>4652</v>
       </c>
       <c r="B152" s="4" t="s">
         <v>1223</v>
@@ -17721,7 +17724,7 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
-        <v>4655</v>
+        <v>4653</v>
       </c>
       <c r="B153" s="4" t="s">
         <v>1225</v>
@@ -17735,7 +17738,7 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
-        <v>4656</v>
+        <v>4654</v>
       </c>
       <c r="B154" s="4" t="s">
         <v>1227</v>
@@ -17763,7 +17766,7 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
-        <v>4657</v>
+        <v>4655</v>
       </c>
       <c r="B156" s="4" t="s">
         <v>1231</v>
@@ -17777,7 +17780,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
-        <v>4658</v>
+        <v>4656</v>
       </c>
       <c r="B157" s="4" t="s">
         <v>1233</v>
@@ -17805,7 +17808,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
-        <v>4659</v>
+        <v>4657</v>
       </c>
       <c r="B159" s="4" t="s">
         <v>1143</v>
@@ -17819,7 +17822,7 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
-        <v>4660</v>
+        <v>4658</v>
       </c>
       <c r="B160" s="4" t="s">
         <v>1145</v>
@@ -17833,7 +17836,7 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
-        <v>4661</v>
+        <v>4659</v>
       </c>
       <c r="B161" s="4" t="s">
         <v>1147</v>
@@ -17861,7 +17864,7 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
-        <v>4662</v>
+        <v>4660</v>
       </c>
       <c r="B163" s="4" t="s">
         <v>1151</v>
@@ -17889,7 +17892,7 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
-        <v>4663</v>
+        <v>4661</v>
       </c>
       <c r="B165" s="4" t="s">
         <v>1155</v>
@@ -17903,7 +17906,7 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
-        <v>4664</v>
+        <v>4662</v>
       </c>
       <c r="B166" s="4" t="s">
         <v>1157</v>
@@ -17917,7 +17920,7 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
-        <v>4665</v>
+        <v>4663</v>
       </c>
       <c r="B167" s="4" t="s">
         <v>1159</v>
@@ -17959,7 +17962,7 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
-        <v>4666</v>
+        <v>4664</v>
       </c>
       <c r="B170" s="4" t="s">
         <v>1165</v>
@@ -17973,7 +17976,7 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
-        <v>4667</v>
+        <v>4665</v>
       </c>
       <c r="B171" s="4" t="s">
         <v>1167</v>
@@ -17987,7 +17990,7 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
-        <v>4995</v>
+        <v>4993</v>
       </c>
       <c r="B172" s="4" t="s">
         <v>1169</v>
@@ -18001,7 +18004,7 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
-        <v>4667</v>
+        <v>4665</v>
       </c>
       <c r="B173" s="4" t="s">
         <v>1171</v>
@@ -18015,7 +18018,7 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
-        <v>4996</v>
+        <v>4994</v>
       </c>
       <c r="B174" s="4" t="s">
         <v>1173</v>
@@ -18043,7 +18046,7 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
-        <v>4997</v>
+        <v>4995</v>
       </c>
       <c r="B176" s="4" t="s">
         <v>1177</v>
@@ -18057,7 +18060,7 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
-        <v>4998</v>
+        <v>4996</v>
       </c>
       <c r="B177" s="4" t="s">
         <v>1179</v>
@@ -18085,7 +18088,7 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
-        <v>4668</v>
+        <v>4666</v>
       </c>
       <c r="B179" s="4" t="s">
         <v>1183</v>
@@ -18127,7 +18130,7 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
-        <v>4669</v>
+        <v>4667</v>
       </c>
       <c r="B182" s="4" t="s">
         <v>1189</v>
@@ -18141,7 +18144,7 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
-        <v>4670</v>
+        <v>4668</v>
       </c>
       <c r="B183" s="4" t="s">
         <v>1191</v>
@@ -18155,7 +18158,7 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
-        <v>4671</v>
+        <v>4669</v>
       </c>
       <c r="B184" s="4" t="s">
         <v>1193</v>
@@ -18169,7 +18172,7 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
-        <v>4672</v>
+        <v>4670</v>
       </c>
       <c r="B185" s="4" t="s">
         <v>1195</v>
@@ -18183,7 +18186,7 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
-        <v>4680</v>
+        <v>4678</v>
       </c>
       <c r="B186" s="4" t="s">
         <v>1197</v>
@@ -18197,7 +18200,7 @@
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
-        <v>4681</v>
+        <v>4679</v>
       </c>
       <c r="B187" s="4" t="s">
         <v>1199</v>
@@ -18211,7 +18214,7 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
-        <v>4682</v>
+        <v>4680</v>
       </c>
       <c r="B188" s="4" t="s">
         <v>1201</v>
@@ -18220,12 +18223,12 @@
         <v>4236</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>4683</v>
+        <v>4681</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
-        <v>4687</v>
+        <v>4685</v>
       </c>
       <c r="B189" s="4" t="s">
         <v>1203</v>
@@ -18239,7 +18242,7 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
-        <v>4688</v>
+        <v>4686</v>
       </c>
       <c r="B190" s="4" t="s">
         <v>754</v>
@@ -18253,7 +18256,7 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
-        <v>4684</v>
+        <v>4682</v>
       </c>
       <c r="B191" s="4" t="s">
         <v>755</v>
@@ -18262,12 +18265,12 @@
         <v>4237</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>4685</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
-        <v>4686</v>
+        <v>4684</v>
       </c>
       <c r="B192" s="4" t="s">
         <v>1207</v>
@@ -18281,7 +18284,7 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
-        <v>4689</v>
+        <v>4687</v>
       </c>
       <c r="B193" s="4" t="s">
         <v>1209</v>
@@ -18295,7 +18298,7 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
-        <v>4694</v>
+        <v>4692</v>
       </c>
       <c r="B194" s="4" t="s">
         <v>1211</v>
@@ -18309,7 +18312,7 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
-        <v>4690</v>
+        <v>4688</v>
       </c>
       <c r="B195" s="4" t="s">
         <v>757</v>
@@ -18323,7 +18326,7 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
-        <v>4695</v>
+        <v>4693</v>
       </c>
       <c r="B196" s="4" t="s">
         <v>759</v>
@@ -18337,7 +18340,7 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
-        <v>4691</v>
+        <v>4689</v>
       </c>
       <c r="B197" s="4" t="s">
         <v>1215</v>
@@ -18351,7 +18354,7 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
-        <v>4696</v>
+        <v>4694</v>
       </c>
       <c r="B198" s="4" t="s">
         <v>1217</v>
@@ -18365,7 +18368,7 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
-        <v>4692</v>
+        <v>4690</v>
       </c>
       <c r="B199" s="4" t="s">
         <v>1219</v>
@@ -18379,7 +18382,7 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
-        <v>4693</v>
+        <v>4691</v>
       </c>
       <c r="B200" s="4" t="s">
         <v>1224</v>
@@ -18393,7 +18396,7 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
-        <v>4697</v>
+        <v>4695</v>
       </c>
       <c r="B201" s="4" t="s">
         <v>1226</v>
@@ -18407,7 +18410,7 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
-        <v>4698</v>
+        <v>4696</v>
       </c>
       <c r="B202" s="4" t="s">
         <v>1228</v>
@@ -18421,7 +18424,7 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
-        <v>4699</v>
+        <v>4697</v>
       </c>
       <c r="B203" s="4" t="s">
         <v>1230</v>
@@ -18435,7 +18438,7 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
-        <v>4700</v>
+        <v>4698</v>
       </c>
       <c r="B204" s="4" t="s">
         <v>1232</v>
@@ -18449,7 +18452,7 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
-        <v>4701</v>
+        <v>4699</v>
       </c>
       <c r="B205" s="4" t="s">
         <v>1234</v>
@@ -18463,7 +18466,7 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
-        <v>4702</v>
+        <v>4700</v>
       </c>
       <c r="B206" s="4" t="s">
         <v>1235</v>
@@ -18477,7 +18480,7 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
-        <v>4703</v>
+        <v>4701</v>
       </c>
       <c r="B207" s="4" t="s">
         <v>1236</v>
@@ -18491,7 +18494,7 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
-        <v>4706</v>
+        <v>4704</v>
       </c>
       <c r="B208" s="4" t="s">
         <v>1237</v>
@@ -18505,7 +18508,7 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
-        <v>4704</v>
+        <v>4702</v>
       </c>
       <c r="B209" s="4" t="s">
         <v>1238</v>
@@ -18519,7 +18522,7 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
-        <v>4705</v>
+        <v>4703</v>
       </c>
       <c r="B210" s="4" t="s">
         <v>761</v>
@@ -18533,7 +18536,7 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
-        <v>4707</v>
+        <v>4705</v>
       </c>
       <c r="B211" s="4" t="s">
         <v>1239</v>
@@ -18547,7 +18550,7 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
-        <v>4708</v>
+        <v>4706</v>
       </c>
       <c r="B212" s="4" t="s">
         <v>1240</v>
@@ -18561,7 +18564,7 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
-        <v>4709</v>
+        <v>4707</v>
       </c>
       <c r="B213" s="4" t="s">
         <v>1241</v>
@@ -18575,7 +18578,7 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
-        <v>4710</v>
+        <v>4708</v>
       </c>
       <c r="B214" s="4" t="s">
         <v>1242</v>
@@ -18589,7 +18592,7 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215" s="4" t="s">
-        <v>4711</v>
+        <v>4709</v>
       </c>
       <c r="B215" s="4" t="s">
         <v>1243</v>
@@ -18603,7 +18606,7 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A216" s="4" t="s">
-        <v>4712</v>
+        <v>4710</v>
       </c>
       <c r="B216" s="4" t="s">
         <v>1244</v>
@@ -18617,7 +18620,7 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
-        <v>4713</v>
+        <v>4711</v>
       </c>
       <c r="B217" s="4" t="s">
         <v>1245</v>
@@ -18631,7 +18634,7 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
-        <v>4714</v>
+        <v>4712</v>
       </c>
       <c r="B218" s="4" t="s">
         <v>1246</v>
@@ -18645,7 +18648,7 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
-        <v>4715</v>
+        <v>4713</v>
       </c>
       <c r="B219" s="4" t="s">
         <v>1247</v>
@@ -18659,7 +18662,7 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
-        <v>4716</v>
+        <v>4714</v>
       </c>
       <c r="B220" s="4" t="s">
         <v>1248</v>
@@ -18673,7 +18676,7 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="B221" s="4" t="s">
         <v>1249</v>
@@ -18687,7 +18690,7 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
-        <v>4718</v>
+        <v>4716</v>
       </c>
       <c r="B222" s="4" t="s">
         <v>1250</v>
@@ -18701,7 +18704,7 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
-        <v>4719</v>
+        <v>4717</v>
       </c>
       <c r="B223" s="4" t="s">
         <v>1251</v>
@@ -18715,7 +18718,7 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
-        <v>4720</v>
+        <v>4718</v>
       </c>
       <c r="B224" s="4" t="s">
         <v>1252</v>
@@ -18729,7 +18732,7 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
-        <v>4721</v>
+        <v>4719</v>
       </c>
       <c r="B225" s="4" t="s">
         <v>1253</v>
@@ -18743,7 +18746,7 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
-        <v>4722</v>
+        <v>4720</v>
       </c>
       <c r="B226" s="4" t="s">
         <v>1254</v>
@@ -18757,7 +18760,7 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
-        <v>4723</v>
+        <v>4721</v>
       </c>
       <c r="B227" s="4" t="s">
         <v>1255</v>
@@ -18771,7 +18774,7 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
-        <v>4724</v>
+        <v>4722</v>
       </c>
       <c r="B228" s="4" t="s">
         <v>1256</v>
@@ -18785,7 +18788,7 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
-        <v>4725</v>
+        <v>4723</v>
       </c>
       <c r="B229" s="4" t="s">
         <v>1257</v>
@@ -18799,7 +18802,7 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
-        <v>4726</v>
+        <v>4724</v>
       </c>
       <c r="B230" s="4" t="s">
         <v>1258</v>
@@ -18813,7 +18816,7 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
-        <v>4727</v>
+        <v>4725</v>
       </c>
       <c r="B231" s="4" t="s">
         <v>1259</v>
@@ -18827,7 +18830,7 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
-        <v>4728</v>
+        <v>4726</v>
       </c>
       <c r="B232" s="4" t="s">
         <v>1260</v>
@@ -18841,7 +18844,7 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
-        <v>4729</v>
+        <v>4727</v>
       </c>
       <c r="B233" s="4" t="s">
         <v>1261</v>
@@ -18855,7 +18858,7 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
-        <v>4730</v>
+        <v>4728</v>
       </c>
       <c r="B234" s="4" t="s">
         <v>1262</v>
@@ -18869,7 +18872,7 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
-        <v>4731</v>
+        <v>4729</v>
       </c>
       <c r="B235" s="4" t="s">
         <v>1263</v>
@@ -18883,7 +18886,7 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
-        <v>4732</v>
+        <v>4730</v>
       </c>
       <c r="B236" s="4" t="s">
         <v>1264</v>
@@ -18897,7 +18900,7 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
-        <v>4733</v>
+        <v>4731</v>
       </c>
       <c r="B237" s="4" t="s">
         <v>1265</v>
@@ -18911,7 +18914,7 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
-        <v>4734</v>
+        <v>4732</v>
       </c>
       <c r="B238" s="4" t="s">
         <v>1266</v>
@@ -18953,7 +18956,7 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
-        <v>4735</v>
+        <v>4733</v>
       </c>
       <c r="B241" s="4" t="s">
         <v>1269</v>
@@ -18967,7 +18970,7 @@
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
-        <v>4736</v>
+        <v>4734</v>
       </c>
       <c r="B242" s="4" t="s">
         <v>1270</v>
@@ -18976,12 +18979,12 @@
         <v>4238</v>
       </c>
       <c r="D242" s="4" t="s">
-        <v>4737</v>
+        <v>4735</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
-        <v>4739</v>
+        <v>4737</v>
       </c>
       <c r="B243" s="4" t="s">
         <v>786</v>
@@ -18990,7 +18993,7 @@
         <v>4239</v>
       </c>
       <c r="D243" s="4" t="s">
-        <v>4738</v>
+        <v>4736</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -19023,7 +19026,7 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
-        <v>4740</v>
+        <v>4738</v>
       </c>
       <c r="B246" s="4" t="s">
         <v>1273</v>
@@ -19037,7 +19040,7 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
-        <v>4741</v>
+        <v>4739</v>
       </c>
       <c r="B247" s="4" t="s">
         <v>1274</v>
@@ -19051,7 +19054,7 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
-        <v>5001</v>
+        <v>4999</v>
       </c>
       <c r="B248" s="4" t="s">
         <v>1275</v>
@@ -19079,7 +19082,7 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
-        <v>4743</v>
+        <v>4741</v>
       </c>
       <c r="B250" s="4" t="s">
         <v>1277</v>
@@ -19093,7 +19096,7 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
-        <v>4744</v>
+        <v>4742</v>
       </c>
       <c r="B251" s="4" t="s">
         <v>789</v>
@@ -19107,7 +19110,7 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
-        <v>4745</v>
+        <v>4743</v>
       </c>
       <c r="B252" s="4" t="s">
         <v>1278</v>
@@ -19121,7 +19124,7 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
-        <v>4746</v>
+        <v>4744</v>
       </c>
       <c r="B253" s="4" t="s">
         <v>791</v>
@@ -19135,7 +19138,7 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
-        <v>4747</v>
+        <v>4745</v>
       </c>
       <c r="B254" s="4" t="s">
         <v>1279</v>
@@ -19163,7 +19166,7 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
-        <v>4748</v>
+        <v>4746</v>
       </c>
       <c r="B256" s="4" t="s">
         <v>1281</v>
@@ -19177,7 +19180,7 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
-        <v>4749</v>
+        <v>4747</v>
       </c>
       <c r="B257" s="4" t="s">
         <v>1282</v>
@@ -19191,7 +19194,7 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
-        <v>4750</v>
+        <v>4748</v>
       </c>
       <c r="B258" s="4" t="s">
         <v>1283</v>
@@ -19205,7 +19208,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
-        <v>4751</v>
+        <v>4749</v>
       </c>
       <c r="B259" s="4" t="s">
         <v>1284</v>
@@ -19219,7 +19222,7 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
-        <v>4752</v>
+        <v>4750</v>
       </c>
       <c r="B260" s="4" t="s">
         <v>798</v>
@@ -19233,7 +19236,7 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
-        <v>4753</v>
+        <v>4751</v>
       </c>
       <c r="B261" s="4" t="s">
         <v>1285</v>
@@ -19247,7 +19250,7 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
-        <v>4754</v>
+        <v>4752</v>
       </c>
       <c r="B262" s="4" t="s">
         <v>1286</v>
@@ -19261,7 +19264,7 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
-        <v>4755</v>
+        <v>4753</v>
       </c>
       <c r="B263" s="4" t="s">
         <v>1287</v>
@@ -19275,7 +19278,7 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
-        <v>4756</v>
+        <v>4754</v>
       </c>
       <c r="B264" s="4" t="s">
         <v>800</v>
@@ -21556,7 +21559,7 @@
     </row>
     <row r="470" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A470" s="4" t="s">
-        <v>4999</v>
+        <v>4997</v>
       </c>
       <c r="B470" s="4" t="s">
         <v>793</v>
@@ -21570,7 +21573,7 @@
     </row>
     <row r="471" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A471" s="4" t="s">
-        <v>4757</v>
+        <v>4755</v>
       </c>
       <c r="B471" s="4" t="s">
         <v>795</v>
@@ -21584,7 +21587,7 @@
     </row>
     <row r="472" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A472" s="4" t="s">
-        <v>4758</v>
+        <v>4756</v>
       </c>
       <c r="B472" s="4" t="s">
         <v>796</v>
@@ -21645,7 +21648,7 @@
     </row>
     <row r="477" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A477" s="4" t="s">
-        <v>4760</v>
+        <v>4758</v>
       </c>
       <c r="B477" s="4" t="s">
         <v>808</v>
@@ -21659,7 +21662,7 @@
     </row>
     <row r="478" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A478" s="4" t="s">
-        <v>4761</v>
+        <v>4759</v>
       </c>
       <c r="B478" s="4" t="s">
         <v>810</v>
@@ -21673,7 +21676,7 @@
     </row>
     <row r="479" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A479" s="4" t="s">
-        <v>4762</v>
+        <v>4760</v>
       </c>
       <c r="B479" s="4" t="s">
         <v>812</v>
@@ -21687,7 +21690,7 @@
     </row>
     <row r="480" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A480" s="4" t="s">
-        <v>4763</v>
+        <v>4761</v>
       </c>
       <c r="B480" s="4" t="s">
         <v>814</v>
@@ -21701,7 +21704,7 @@
     </row>
     <row r="481" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A481" s="4" t="s">
-        <v>4764</v>
+        <v>4762</v>
       </c>
       <c r="B481" s="4" t="s">
         <v>816</v>
@@ -21715,7 +21718,7 @@
     </row>
     <row r="482" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A482" s="4" t="s">
-        <v>4765</v>
+        <v>4763</v>
       </c>
       <c r="B482" s="4" t="s">
         <v>817</v>
@@ -21729,7 +21732,7 @@
     </row>
     <row r="483" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A483" s="4" t="s">
-        <v>4766</v>
+        <v>4764</v>
       </c>
       <c r="B483" s="4" t="s">
         <v>818</v>
@@ -21743,7 +21746,7 @@
     </row>
     <row r="484" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A484" s="4" t="s">
-        <v>4759</v>
+        <v>4757</v>
       </c>
       <c r="B484" s="4" t="s">
         <v>820</v>
@@ -21757,7 +21760,7 @@
     </row>
     <row r="485" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A485" s="4" t="s">
-        <v>4767</v>
+        <v>4765</v>
       </c>
       <c r="B485" s="4" t="s">
         <v>822</v>
@@ -21771,7 +21774,7 @@
     </row>
     <row r="486" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A486" s="4" t="s">
-        <v>4768</v>
+        <v>4766</v>
       </c>
       <c r="B486" s="4" t="s">
         <v>824</v>
@@ -21785,7 +21788,7 @@
     </row>
     <row r="487" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A487" s="4" t="s">
-        <v>4769</v>
+        <v>4767</v>
       </c>
       <c r="B487" s="4" t="s">
         <v>825</v>
@@ -21822,12 +21825,12 @@
         <v>4267</v>
       </c>
       <c r="D489" s="4" t="s">
-        <v>4984</v>
+        <v>4982</v>
       </c>
     </row>
     <row r="490" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A490" s="4" t="s">
-        <v>4981</v>
+        <v>4979</v>
       </c>
       <c r="B490" s="4" t="s">
         <v>833</v>
@@ -21836,12 +21839,12 @@
         <v>4268</v>
       </c>
       <c r="D490" s="4" t="s">
-        <v>4983</v>
+        <v>4981</v>
       </c>
     </row>
     <row r="491" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A491" s="4" t="s">
-        <v>4982</v>
+        <v>4980</v>
       </c>
       <c r="B491" s="4" t="s">
         <v>835</v>
@@ -21864,7 +21867,7 @@
         <v>4270</v>
       </c>
       <c r="D492" s="4" t="s">
-        <v>4985</v>
+        <v>4983</v>
       </c>
     </row>
     <row r="493" spans="1:4" x14ac:dyDescent="0.25">
@@ -21878,7 +21881,7 @@
         <v>4271</v>
       </c>
       <c r="D493" s="4" t="s">
-        <v>4987</v>
+        <v>4985</v>
       </c>
     </row>
     <row r="494" spans="1:4" x14ac:dyDescent="0.25">
@@ -21892,7 +21895,7 @@
         <v>4272</v>
       </c>
       <c r="D494" s="4" t="s">
-        <v>4988</v>
+        <v>4986</v>
       </c>
     </row>
     <row r="495" spans="1:4" x14ac:dyDescent="0.25">
@@ -21906,7 +21909,7 @@
         <v>4273</v>
       </c>
       <c r="D495" s="4" t="s">
-        <v>4989</v>
+        <v>4987</v>
       </c>
     </row>
     <row r="496" spans="1:4" x14ac:dyDescent="0.25">
@@ -21920,7 +21923,7 @@
         <v>4274</v>
       </c>
       <c r="D496" s="4" t="s">
-        <v>4986</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="497" spans="1:4" x14ac:dyDescent="0.25">
@@ -21934,7 +21937,7 @@
         <v>4275</v>
       </c>
       <c r="D497" s="4" t="s">
-        <v>4990</v>
+        <v>4988</v>
       </c>
     </row>
     <row r="498" spans="1:4" x14ac:dyDescent="0.25">
@@ -21948,12 +21951,12 @@
         <v>4276</v>
       </c>
       <c r="D498" s="4" t="s">
-        <v>4991</v>
+        <v>4989</v>
       </c>
     </row>
     <row r="499" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A499" s="4" t="s">
-        <v>4774</v>
+        <v>4772</v>
       </c>
       <c r="B499" s="4" t="s">
         <v>848</v>
@@ -21962,7 +21965,7 @@
         <v>4277</v>
       </c>
       <c r="D499" s="4" t="s">
-        <v>4770</v>
+        <v>4768</v>
       </c>
     </row>
     <row r="500" spans="1:4" x14ac:dyDescent="0.25">
@@ -21981,7 +21984,7 @@
     </row>
     <row r="501" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A501" s="4" t="s">
-        <v>4775</v>
+        <v>4773</v>
       </c>
       <c r="B501" s="4" t="s">
         <v>871</v>
@@ -22009,7 +22012,7 @@
     </row>
     <row r="503" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A503" s="4" t="s">
-        <v>4776</v>
+        <v>4774</v>
       </c>
       <c r="B503" s="4" t="s">
         <v>876</v>
@@ -22023,7 +22026,7 @@
     </row>
     <row r="504" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A504" s="4" t="s">
-        <v>4777</v>
+        <v>4775</v>
       </c>
       <c r="B504" s="4" t="s">
         <v>878</v>
@@ -22051,7 +22054,7 @@
     </row>
     <row r="506" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A506" s="4" t="s">
-        <v>4772</v>
+        <v>4770</v>
       </c>
       <c r="B506" s="4" t="s">
         <v>882</v>
@@ -22060,7 +22063,7 @@
         <v>4284</v>
       </c>
       <c r="D506" s="4" t="s">
-        <v>4771</v>
+        <v>4769</v>
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
@@ -22079,7 +22082,7 @@
     </row>
     <row r="508" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A508" s="4" t="s">
-        <v>4778</v>
+        <v>4776</v>
       </c>
       <c r="B508" s="4" t="s">
         <v>886</v>
@@ -22093,7 +22096,7 @@
     </row>
     <row r="509" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A509" s="4" t="s">
-        <v>4779</v>
+        <v>4777</v>
       </c>
       <c r="B509" s="4" t="s">
         <v>1663</v>
@@ -22107,7 +22110,7 @@
     </row>
     <row r="510" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A510" s="4" t="s">
-        <v>4780</v>
+        <v>4778</v>
       </c>
       <c r="B510" s="4" t="s">
         <v>890</v>
@@ -22121,7 +22124,7 @@
     </row>
     <row r="511" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A511" s="4" t="s">
-        <v>4781</v>
+        <v>4779</v>
       </c>
       <c r="B511" s="4" t="s">
         <v>891</v>
@@ -22135,7 +22138,7 @@
     </row>
     <row r="512" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A512" s="4" t="s">
-        <v>4782</v>
+        <v>4780</v>
       </c>
       <c r="B512" s="4" t="s">
         <v>892</v>
@@ -22149,7 +22152,7 @@
     </row>
     <row r="513" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A513" s="4" t="s">
-        <v>4783</v>
+        <v>4781</v>
       </c>
       <c r="B513" s="4" t="s">
         <v>893</v>
@@ -22163,7 +22166,7 @@
     </row>
     <row r="514" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A514" s="4" t="s">
-        <v>4784</v>
+        <v>4782</v>
       </c>
       <c r="B514" s="4" t="s">
         <v>895</v>
@@ -22177,7 +22180,7 @@
     </row>
     <row r="515" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A515" s="4" t="s">
-        <v>4785</v>
+        <v>4783</v>
       </c>
       <c r="B515" s="4" t="s">
         <v>896</v>
@@ -22191,7 +22194,7 @@
     </row>
     <row r="516" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A516" s="4" t="s">
-        <v>4786</v>
+        <v>4784</v>
       </c>
       <c r="B516" s="4" t="s">
         <v>897</v>
@@ -22205,7 +22208,7 @@
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A517" s="4" t="s">
-        <v>4787</v>
+        <v>4785</v>
       </c>
       <c r="B517" s="4" t="s">
         <v>902</v>
@@ -22233,7 +22236,7 @@
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A519" s="4" t="s">
-        <v>4788</v>
+        <v>4786</v>
       </c>
       <c r="B519" s="4" t="s">
         <v>906</v>
@@ -22247,7 +22250,7 @@
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A520" s="4" t="s">
-        <v>4789</v>
+        <v>4787</v>
       </c>
       <c r="B520" s="4" t="s">
         <v>908</v>
@@ -22261,7 +22264,7 @@
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A521" s="4" t="s">
-        <v>4790</v>
+        <v>4788</v>
       </c>
       <c r="B521" s="4" t="s">
         <v>910</v>
@@ -22275,7 +22278,7 @@
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A522" s="4" t="s">
-        <v>4791</v>
+        <v>4789</v>
       </c>
       <c r="B522" s="4" t="s">
         <v>911</v>
@@ -22303,7 +22306,7 @@
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A524" s="4" t="s">
-        <v>4792</v>
+        <v>4790</v>
       </c>
       <c r="B524" s="4" t="s">
         <v>915</v>
@@ -22317,7 +22320,7 @@
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A525" s="4" t="s">
-        <v>4793</v>
+        <v>4791</v>
       </c>
       <c r="B525" s="4" t="s">
         <v>916</v>
@@ -22331,7 +22334,7 @@
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A526" s="4" t="s">
-        <v>4794</v>
+        <v>4792</v>
       </c>
       <c r="B526" s="4" t="s">
         <v>918</v>
@@ -22359,7 +22362,7 @@
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A528" s="4" t="s">
-        <v>4795</v>
+        <v>4793</v>
       </c>
       <c r="B528" s="4" t="s">
         <v>922</v>
@@ -22373,7 +22376,7 @@
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A529" s="4" t="s">
-        <v>4796</v>
+        <v>4794</v>
       </c>
       <c r="B529" s="4" t="s">
         <v>924</v>
@@ -22401,7 +22404,7 @@
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" s="4" t="s">
-        <v>4797</v>
+        <v>4795</v>
       </c>
       <c r="B531" s="4" t="s">
         <v>928</v>
@@ -22415,7 +22418,7 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" s="4" t="s">
-        <v>4798</v>
+        <v>4796</v>
       </c>
       <c r="B532" s="4" t="s">
         <v>930</v>
@@ -22429,7 +22432,7 @@
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" s="4" t="s">
-        <v>4799</v>
+        <v>4797</v>
       </c>
       <c r="B533" s="4" t="s">
         <v>931</v>
@@ -22443,7 +22446,7 @@
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" s="4" t="s">
-        <v>4800</v>
+        <v>4798</v>
       </c>
       <c r="B534" s="4" t="s">
         <v>933</v>
@@ -22457,7 +22460,7 @@
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" s="4" t="s">
-        <v>4801</v>
+        <v>4799</v>
       </c>
       <c r="B535" s="4" t="s">
         <v>934</v>
@@ -22471,7 +22474,7 @@
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" s="4" t="s">
-        <v>4802</v>
+        <v>4800</v>
       </c>
       <c r="B536" s="4" t="s">
         <v>936</v>
@@ -22485,7 +22488,7 @@
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" s="4" t="s">
-        <v>4803</v>
+        <v>4801</v>
       </c>
       <c r="B537" s="4" t="s">
         <v>937</v>
@@ -22499,7 +22502,7 @@
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A538" s="4" t="s">
-        <v>4804</v>
+        <v>4802</v>
       </c>
       <c r="B538" s="4" t="s">
         <v>938</v>
@@ -22513,7 +22516,7 @@
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A539" s="4" t="s">
-        <v>4805</v>
+        <v>4803</v>
       </c>
       <c r="B539" s="4" t="s">
         <v>939</v>
@@ -22527,7 +22530,7 @@
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A540" s="4" t="s">
-        <v>4806</v>
+        <v>4804</v>
       </c>
       <c r="B540" s="4" t="s">
         <v>940</v>
@@ -22541,7 +22544,7 @@
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A541" s="4" t="s">
-        <v>4807</v>
+        <v>4805</v>
       </c>
       <c r="B541" s="4" t="s">
         <v>942</v>
@@ -22555,7 +22558,7 @@
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A542" s="4" t="s">
-        <v>4808</v>
+        <v>4806</v>
       </c>
       <c r="B542" s="4" t="s">
         <v>943</v>
@@ -22583,7 +22586,7 @@
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A544" s="4" t="s">
-        <v>4809</v>
+        <v>4807</v>
       </c>
       <c r="B544" s="4" t="s">
         <v>947</v>
@@ -22611,7 +22614,7 @@
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A546" s="4" t="s">
-        <v>4810</v>
+        <v>4808</v>
       </c>
       <c r="B546" s="4" t="s">
         <v>951</v>
@@ -22667,7 +22670,7 @@
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A550" s="4" t="s">
-        <v>4811</v>
+        <v>4809</v>
       </c>
       <c r="B550" s="4" t="s">
         <v>959</v>
@@ -22695,7 +22698,7 @@
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A552" s="4" t="s">
-        <v>4812</v>
+        <v>4810</v>
       </c>
       <c r="B552" s="4" t="s">
         <v>962</v>
@@ -22737,7 +22740,7 @@
     </row>
     <row r="555" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A555" s="4" t="s">
-        <v>4813</v>
+        <v>4811</v>
       </c>
       <c r="B555" s="4" t="s">
         <v>968</v>
@@ -22765,7 +22768,7 @@
     </row>
     <row r="557" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A557" s="4" t="s">
-        <v>4814</v>
+        <v>4812</v>
       </c>
       <c r="B557" s="4" t="s">
         <v>971</v>
@@ -22779,7 +22782,7 @@
     </row>
     <row r="558" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A558" s="4" t="s">
-        <v>4815</v>
+        <v>4813</v>
       </c>
       <c r="B558" s="4" t="s">
         <v>973</v>
@@ -22793,7 +22796,7 @@
     </row>
     <row r="559" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A559" s="4" t="s">
-        <v>4816</v>
+        <v>4814</v>
       </c>
       <c r="B559" s="4" t="s">
         <v>975</v>
@@ -22807,7 +22810,7 @@
     </row>
     <row r="560" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A560" s="4" t="s">
-        <v>4817</v>
+        <v>4815</v>
       </c>
       <c r="B560" s="4" t="s">
         <v>976</v>
@@ -22821,7 +22824,7 @@
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A561" s="4" t="s">
-        <v>4818</v>
+        <v>4816</v>
       </c>
       <c r="B561" s="4" t="s">
         <v>977</v>
@@ -22835,7 +22838,7 @@
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A562" s="4" t="s">
-        <v>4819</v>
+        <v>4817</v>
       </c>
       <c r="B562" s="4" t="s">
         <v>978</v>
@@ -22849,7 +22852,7 @@
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A563" s="4" t="s">
-        <v>4820</v>
+        <v>4818</v>
       </c>
       <c r="B563" s="4" t="s">
         <v>979</v>
@@ -22863,7 +22866,7 @@
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A564" s="4" t="s">
-        <v>4821</v>
+        <v>4819</v>
       </c>
       <c r="B564" s="4" t="s">
         <v>980</v>
@@ -22877,7 +22880,7 @@
     </row>
     <row r="565" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A565" s="4" t="s">
-        <v>4822</v>
+        <v>4820</v>
       </c>
       <c r="B565" s="4" t="s">
         <v>981</v>
@@ -22891,7 +22894,7 @@
     </row>
     <row r="566" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A566" s="4" t="s">
-        <v>4823</v>
+        <v>4821</v>
       </c>
       <c r="B566" s="4" t="s">
         <v>982</v>
@@ -22905,7 +22908,7 @@
     </row>
     <row r="567" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A567" s="4" t="s">
-        <v>4824</v>
+        <v>4822</v>
       </c>
       <c r="B567" s="4" t="s">
         <v>983</v>
@@ -22947,7 +22950,7 @@
     </row>
     <row r="570" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A570" s="4" t="s">
-        <v>4773</v>
+        <v>4771</v>
       </c>
       <c r="B570" s="4" t="s">
         <v>988</v>
@@ -23017,7 +23020,7 @@
     </row>
     <row r="575" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A575" s="4" t="s">
-        <v>4825</v>
+        <v>4823</v>
       </c>
       <c r="B575" s="4" t="s">
         <v>997</v>
@@ -23031,7 +23034,7 @@
     </row>
     <row r="576" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A576" s="4" t="s">
-        <v>4826</v>
+        <v>4824</v>
       </c>
       <c r="B576" s="4" t="s">
         <v>999</v>
@@ -23045,7 +23048,7 @@
     </row>
     <row r="577" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A577" s="4" t="s">
-        <v>4827</v>
+        <v>4825</v>
       </c>
       <c r="B577" s="4" t="s">
         <v>1001</v>
@@ -23101,7 +23104,7 @@
     </row>
     <row r="581" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A581" s="4" t="s">
-        <v>4828</v>
+        <v>4826</v>
       </c>
       <c r="B581" s="4" t="s">
         <v>1009</v>
@@ -23115,7 +23118,7 @@
     </row>
     <row r="582" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A582" s="4" t="s">
-        <v>4829</v>
+        <v>4827</v>
       </c>
       <c r="B582" s="4" t="s">
         <v>1010</v>
@@ -23129,7 +23132,7 @@
     </row>
     <row r="583" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A583" s="4" t="s">
-        <v>4830</v>
+        <v>4828</v>
       </c>
       <c r="B583" s="4" t="s">
         <v>1011</v>
@@ -23143,7 +23146,7 @@
     </row>
     <row r="584" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A584" s="4" t="s">
-        <v>4831</v>
+        <v>4829</v>
       </c>
       <c r="B584" s="4" t="s">
         <v>1012</v>
@@ -23157,7 +23160,7 @@
     </row>
     <row r="585" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A585" s="4" t="s">
-        <v>4832</v>
+        <v>4830</v>
       </c>
       <c r="B585" s="4" t="s">
         <v>1013</v>
@@ -23171,7 +23174,7 @@
     </row>
     <row r="586" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A586" s="4" t="s">
-        <v>4833</v>
+        <v>4831</v>
       </c>
       <c r="B586" s="4" t="s">
         <v>1014</v>
@@ -23185,7 +23188,7 @@
     </row>
     <row r="587" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A587" s="4" t="s">
-        <v>4834</v>
+        <v>4832</v>
       </c>
       <c r="B587" s="4" t="s">
         <v>1015</v>
@@ -23199,7 +23202,7 @@
     </row>
     <row r="588" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A588" s="4" t="s">
-        <v>4835</v>
+        <v>4833</v>
       </c>
       <c r="B588" s="4" t="s">
         <v>1017</v>
@@ -23227,7 +23230,7 @@
     </row>
     <row r="590" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A590" s="4" t="s">
-        <v>4836</v>
+        <v>4834</v>
       </c>
       <c r="B590" s="4" t="s">
         <v>1020</v>
@@ -23255,7 +23258,7 @@
     </row>
     <row r="592" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A592" s="4" t="s">
-        <v>4837</v>
+        <v>4835</v>
       </c>
       <c r="B592" s="4" t="s">
         <v>1023</v>
@@ -23269,7 +23272,7 @@
     </row>
     <row r="593" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A593" s="4" t="s">
-        <v>4838</v>
+        <v>4836</v>
       </c>
       <c r="B593" s="4" t="s">
         <v>2826</v>
@@ -23283,7 +23286,7 @@
     </row>
     <row r="594" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A594" s="4" t="s">
-        <v>4839</v>
+        <v>4837</v>
       </c>
       <c r="B594" s="4" t="s">
         <v>1024</v>
@@ -23297,7 +23300,7 @@
     </row>
     <row r="595" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A595" s="4" t="s">
-        <v>4840</v>
+        <v>4838</v>
       </c>
       <c r="B595" s="4" t="s">
         <v>1026</v>
@@ -23311,7 +23314,7 @@
     </row>
     <row r="596" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A596" s="4" t="s">
-        <v>4841</v>
+        <v>4839</v>
       </c>
       <c r="B596" s="4" t="s">
         <v>1027</v>
@@ -23325,7 +23328,7 @@
     </row>
     <row r="597" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A597" s="4" t="s">
-        <v>4842</v>
+        <v>4840</v>
       </c>
       <c r="B597" s="4" t="s">
         <v>1028</v>
@@ -23482,7 +23485,7 @@
     </row>
     <row r="611" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A611" s="4" t="s">
-        <v>4844</v>
+        <v>4842</v>
       </c>
       <c r="B611" s="4" t="s">
         <v>763</v>
@@ -23496,7 +23499,7 @@
     </row>
     <row r="612" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A612" s="4" t="s">
-        <v>5000</v>
+        <v>4998</v>
       </c>
       <c r="B612" s="4" t="s">
         <v>1859</v>
@@ -23510,7 +23513,7 @@
     </row>
     <row r="613" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A613" s="4" t="s">
-        <v>4843</v>
+        <v>4841</v>
       </c>
       <c r="B613" s="4" t="s">
         <v>765</v>
@@ -23524,7 +23527,7 @@
     </row>
     <row r="614" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A614" s="4" t="s">
-        <v>4845</v>
+        <v>4843</v>
       </c>
       <c r="B614" s="4" t="s">
         <v>1860</v>
@@ -23538,7 +23541,7 @@
     </row>
     <row r="615" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A615" s="4" t="s">
-        <v>4846</v>
+        <v>4844</v>
       </c>
       <c r="B615" s="4" t="s">
         <v>766</v>
@@ -23552,7 +23555,7 @@
     </row>
     <row r="616" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A616" s="4" t="s">
-        <v>4847</v>
+        <v>4845</v>
       </c>
       <c r="B616" s="4" t="s">
         <v>768</v>
@@ -23566,7 +23569,7 @@
     </row>
     <row r="617" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A617" s="4" t="s">
-        <v>4742</v>
+        <v>4740</v>
       </c>
       <c r="B617" s="4" t="s">
         <v>1862</v>
@@ -23580,7 +23583,7 @@
     </row>
     <row r="618" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A618" s="4" t="s">
-        <v>4848</v>
+        <v>4846</v>
       </c>
       <c r="B618" s="4" t="s">
         <v>1863</v>
@@ -23594,7 +23597,7 @@
     </row>
     <row r="619" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A619" s="4" t="s">
-        <v>4849</v>
+        <v>4847</v>
       </c>
       <c r="B619" s="4" t="s">
         <v>1864</v>
@@ -23608,7 +23611,7 @@
     </row>
     <row r="620" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A620" s="4" t="s">
-        <v>4850</v>
+        <v>4848</v>
       </c>
       <c r="B620" s="4" t="s">
         <v>1865</v>
@@ -23622,7 +23625,7 @@
     </row>
     <row r="621" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A621" s="4" t="s">
-        <v>4851</v>
+        <v>4849</v>
       </c>
       <c r="B621" s="4" t="s">
         <v>1866</v>
@@ -23636,7 +23639,7 @@
     </row>
     <row r="622" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A622" s="4" t="s">
-        <v>4852</v>
+        <v>4850</v>
       </c>
       <c r="B622" s="4" t="s">
         <v>769</v>
@@ -23650,7 +23653,7 @@
     </row>
     <row r="623" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A623" s="4" t="s">
-        <v>4853</v>
+        <v>4851</v>
       </c>
       <c r="B623" s="4" t="s">
         <v>1867</v>
@@ -23664,7 +23667,7 @@
     </row>
     <row r="624" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A624" s="4" t="s">
-        <v>4854</v>
+        <v>4852</v>
       </c>
       <c r="B624" s="4" t="s">
         <v>1868</v>
@@ -23678,7 +23681,7 @@
     </row>
     <row r="625" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A625" s="4" t="s">
-        <v>4855</v>
+        <v>4853</v>
       </c>
       <c r="B625" s="4" t="s">
         <v>1869</v>
@@ -23692,7 +23695,7 @@
     </row>
     <row r="626" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A626" s="4" t="s">
-        <v>4856</v>
+        <v>4854</v>
       </c>
       <c r="B626" s="4" t="s">
         <v>1870</v>
@@ -23706,7 +23709,7 @@
     </row>
     <row r="627" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A627" s="4" t="s">
-        <v>4857</v>
+        <v>4855</v>
       </c>
       <c r="B627" s="4" t="s">
         <v>1871</v>
@@ -23720,7 +23723,7 @@
     </row>
     <row r="628" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A628" s="4" t="s">
-        <v>4858</v>
+        <v>4856</v>
       </c>
       <c r="B628" s="4" t="s">
         <v>1872</v>
@@ -23734,7 +23737,7 @@
     </row>
     <row r="629" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A629" s="4" t="s">
-        <v>4861</v>
+        <v>4859</v>
       </c>
       <c r="B629" s="4" t="s">
         <v>1873</v>
@@ -23748,7 +23751,7 @@
     </row>
     <row r="630" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A630" s="4" t="s">
-        <v>4862</v>
+        <v>4860</v>
       </c>
       <c r="B630" s="4" t="s">
         <v>1874</v>
@@ -23762,7 +23765,7 @@
     </row>
     <row r="631" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A631" s="4" t="s">
-        <v>4863</v>
+        <v>4861</v>
       </c>
       <c r="B631" s="4" t="s">
         <v>1875</v>
@@ -23776,7 +23779,7 @@
     </row>
     <row r="632" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A632" s="4" t="s">
-        <v>4864</v>
+        <v>4862</v>
       </c>
       <c r="B632" s="4" t="s">
         <v>1876</v>
@@ -23790,7 +23793,7 @@
     </row>
     <row r="633" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A633" s="4" t="s">
-        <v>4865</v>
+        <v>4863</v>
       </c>
       <c r="B633" s="4" t="s">
         <v>1877</v>
@@ -23804,7 +23807,7 @@
     </row>
     <row r="634" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A634" s="4" t="s">
-        <v>4866</v>
+        <v>4864</v>
       </c>
       <c r="B634" s="4" t="s">
         <v>1878</v>
@@ -23818,7 +23821,7 @@
     </row>
     <row r="635" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A635" s="4" t="s">
-        <v>4867</v>
+        <v>4865</v>
       </c>
       <c r="B635" s="4" t="s">
         <v>1879</v>
@@ -23832,7 +23835,7 @@
     </row>
     <row r="636" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A636" s="4" t="s">
-        <v>4868</v>
+        <v>4866</v>
       </c>
       <c r="B636" s="4" t="s">
         <v>1880</v>
@@ -23846,7 +23849,7 @@
     </row>
     <row r="637" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A637" s="4" t="s">
-        <v>4869</v>
+        <v>4867</v>
       </c>
       <c r="B637" s="4" t="s">
         <v>770</v>
@@ -23860,7 +23863,7 @@
     </row>
     <row r="638" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A638" s="4" t="s">
-        <v>4870</v>
+        <v>4868</v>
       </c>
       <c r="B638" s="4" t="s">
         <v>1881</v>
@@ -23874,7 +23877,7 @@
     </row>
     <row r="639" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A639" s="4" t="s">
-        <v>4871</v>
+        <v>4869</v>
       </c>
       <c r="B639" s="4" t="s">
         <v>1882</v>
@@ -23888,7 +23891,7 @@
     </row>
     <row r="640" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A640" s="4" t="s">
-        <v>4872</v>
+        <v>4870</v>
       </c>
       <c r="B640" s="4" t="s">
         <v>1883</v>
@@ -23902,7 +23905,7 @@
     </row>
     <row r="641" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A641" s="4" t="s">
-        <v>4873</v>
+        <v>4871</v>
       </c>
       <c r="B641" s="4" t="s">
         <v>1884</v>
@@ -23916,7 +23919,7 @@
     </row>
     <row r="642" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A642" s="4" t="s">
-        <v>4874</v>
+        <v>4872</v>
       </c>
       <c r="B642" s="4" t="s">
         <v>1885</v>
@@ -23930,7 +23933,7 @@
     </row>
     <row r="643" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A643" s="4" t="s">
-        <v>4875</v>
+        <v>4873</v>
       </c>
       <c r="B643" s="4" t="s">
         <v>1886</v>
@@ -23944,7 +23947,7 @@
     </row>
     <row r="644" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A644" s="4" t="s">
-        <v>4876</v>
+        <v>4874</v>
       </c>
       <c r="B644" s="4" t="s">
         <v>772</v>
@@ -23958,7 +23961,7 @@
     </row>
     <row r="645" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A645" s="4" t="s">
-        <v>4877</v>
+        <v>4875</v>
       </c>
       <c r="B645" s="4" t="s">
         <v>1887</v>
@@ -23972,7 +23975,7 @@
     </row>
     <row r="646" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A646" s="4" t="s">
-        <v>4878</v>
+        <v>4876</v>
       </c>
       <c r="B646" s="4" t="s">
         <v>1888</v>
@@ -23986,7 +23989,7 @@
     </row>
     <row r="647" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A647" s="4" t="s">
-        <v>4879</v>
+        <v>4877</v>
       </c>
       <c r="B647" s="4" t="s">
         <v>1889</v>
@@ -24000,7 +24003,7 @@
     </row>
     <row r="648" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A648" s="4" t="s">
-        <v>4880</v>
+        <v>4878</v>
       </c>
       <c r="B648" s="4" t="s">
         <v>1890</v>
@@ -24014,7 +24017,7 @@
     </row>
     <row r="649" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A649" s="4" t="s">
-        <v>4881</v>
+        <v>4879</v>
       </c>
       <c r="B649" s="4" t="s">
         <v>1891</v>
@@ -24028,7 +24031,7 @@
     </row>
     <row r="650" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A650" s="4" t="s">
-        <v>4882</v>
+        <v>4880</v>
       </c>
       <c r="B650" s="4" t="s">
         <v>1892</v>
@@ -24042,7 +24045,7 @@
     </row>
     <row r="651" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A651" s="4" t="s">
-        <v>4883</v>
+        <v>4881</v>
       </c>
       <c r="B651" s="4" t="s">
         <v>1893</v>
@@ -24056,7 +24059,7 @@
     </row>
     <row r="652" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A652" s="4" t="s">
-        <v>4884</v>
+        <v>4882</v>
       </c>
       <c r="B652" s="4" t="s">
         <v>1894</v>
@@ -24070,7 +24073,7 @@
     </row>
     <row r="653" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A653" s="4" t="s">
-        <v>4885</v>
+        <v>4883</v>
       </c>
       <c r="B653" s="4" t="s">
         <v>1895</v>
@@ -24084,7 +24087,7 @@
     </row>
     <row r="654" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A654" s="4" t="s">
-        <v>4886</v>
+        <v>4884</v>
       </c>
       <c r="B654" s="4" t="s">
         <v>1896</v>
@@ -24098,7 +24101,7 @@
     </row>
     <row r="655" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A655" s="4" t="s">
-        <v>4887</v>
+        <v>4885</v>
       </c>
       <c r="B655" s="4" t="s">
         <v>1897</v>
@@ -24112,7 +24115,7 @@
     </row>
     <row r="656" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A656" s="4" t="s">
-        <v>4888</v>
+        <v>4886</v>
       </c>
       <c r="B656" s="4" t="s">
         <v>1898</v>
@@ -24126,7 +24129,7 @@
     </row>
     <row r="657" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A657" s="4" t="s">
-        <v>4889</v>
+        <v>4887</v>
       </c>
       <c r="B657" s="4" t="s">
         <v>1899</v>
@@ -24140,7 +24143,7 @@
     </row>
     <row r="658" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A658" s="4" t="s">
-        <v>4890</v>
+        <v>4888</v>
       </c>
       <c r="B658" s="4" t="s">
         <v>1900</v>
@@ -24154,7 +24157,7 @@
     </row>
     <row r="659" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A659" s="4" t="s">
-        <v>4891</v>
+        <v>4889</v>
       </c>
       <c r="B659" s="4" t="s">
         <v>1901</v>
@@ -24168,7 +24171,7 @@
     </row>
     <row r="660" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A660" s="4" t="s">
-        <v>4892</v>
+        <v>4890</v>
       </c>
       <c r="B660" s="4" t="s">
         <v>1902</v>
@@ -24182,7 +24185,7 @@
     </row>
     <row r="661" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A661" s="4" t="s">
-        <v>4893</v>
+        <v>4891</v>
       </c>
       <c r="B661" s="4" t="s">
         <v>774</v>
@@ -24196,7 +24199,7 @@
     </row>
     <row r="662" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A662" s="4" t="s">
-        <v>4859</v>
+        <v>4857</v>
       </c>
       <c r="B662" s="4" t="s">
         <v>1903</v>
@@ -24210,7 +24213,7 @@
     </row>
     <row r="663" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A663" s="4" t="s">
-        <v>4860</v>
+        <v>4858</v>
       </c>
       <c r="B663" s="4" t="s">
         <v>1904</v>
@@ -24224,7 +24227,7 @@
     </row>
     <row r="664" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A664" s="4" t="s">
-        <v>4894</v>
+        <v>4892</v>
       </c>
       <c r="B664" s="4" t="s">
         <v>1905</v>
@@ -24238,7 +24241,7 @@
     </row>
     <row r="665" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A665" s="4" t="s">
-        <v>4895</v>
+        <v>4893</v>
       </c>
       <c r="B665" s="4" t="s">
         <v>1906</v>
@@ -24252,7 +24255,7 @@
     </row>
     <row r="666" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A666" s="4" t="s">
-        <v>4896</v>
+        <v>4894</v>
       </c>
       <c r="B666" s="4" t="s">
         <v>1907</v>
@@ -24266,7 +24269,7 @@
     </row>
     <row r="667" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A667" s="4" t="s">
-        <v>4897</v>
+        <v>4895</v>
       </c>
       <c r="B667" s="4" t="s">
         <v>1908</v>
@@ -24280,7 +24283,7 @@
     </row>
     <row r="668" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A668" s="4" t="s">
-        <v>4898</v>
+        <v>4896</v>
       </c>
       <c r="B668" s="4" t="s">
         <v>1909</v>
@@ -24459,7 +24462,7 @@
     </row>
     <row r="684" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A684" s="4" t="s">
-        <v>4899</v>
+        <v>4897</v>
       </c>
       <c r="B684" s="4" t="s">
         <v>1923</v>
@@ -24473,7 +24476,7 @@
     </row>
     <row r="685" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A685" s="4" t="s">
-        <v>4901</v>
+        <v>4899</v>
       </c>
       <c r="B685" s="4" t="s">
         <v>1924</v>
@@ -24487,7 +24490,7 @@
     </row>
     <row r="686" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A686" s="4" t="s">
-        <v>4902</v>
+        <v>4900</v>
       </c>
       <c r="B686" s="4" t="s">
         <v>1925</v>
@@ -24501,7 +24504,7 @@
     </row>
     <row r="687" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A687" s="4" t="s">
-        <v>4903</v>
+        <v>4901</v>
       </c>
       <c r="B687" s="4" t="s">
         <v>1926</v>
@@ -24515,7 +24518,7 @@
     </row>
     <row r="688" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A688" s="4" t="s">
-        <v>4904</v>
+        <v>4902</v>
       </c>
       <c r="B688" s="4" t="s">
         <v>1927</v>
@@ -24529,7 +24532,7 @@
     </row>
     <row r="689" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A689" s="4" t="s">
-        <v>4905</v>
+        <v>4903</v>
       </c>
       <c r="B689" s="4" t="s">
         <v>1046</v>
@@ -24543,7 +24546,7 @@
     </row>
     <row r="690" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A690" s="4" t="s">
-        <v>4906</v>
+        <v>4904</v>
       </c>
       <c r="B690" s="4" t="s">
         <v>1928</v>
@@ -24557,7 +24560,7 @@
     </row>
     <row r="691" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A691" s="4" t="s">
-        <v>4907</v>
+        <v>4905</v>
       </c>
       <c r="B691" s="4" t="s">
         <v>1929</v>
@@ -24571,7 +24574,7 @@
     </row>
     <row r="692" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A692" s="4" t="s">
-        <v>4908</v>
+        <v>4906</v>
       </c>
       <c r="B692" s="4" t="s">
         <v>1930</v>
@@ -24585,7 +24588,7 @@
     </row>
     <row r="693" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A693" s="4" t="s">
-        <v>4909</v>
+        <v>4907</v>
       </c>
       <c r="B693" s="4" t="s">
         <v>1931</v>
@@ -24599,7 +24602,7 @@
     </row>
     <row r="694" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A694" s="4" t="s">
-        <v>4910</v>
+        <v>4908</v>
       </c>
       <c r="B694" s="4" t="s">
         <v>1932</v>
@@ -24613,7 +24616,7 @@
     </row>
     <row r="695" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A695" s="4" t="s">
-        <v>4911</v>
+        <v>4909</v>
       </c>
       <c r="B695" s="4" t="s">
         <v>1933</v>
@@ -24622,12 +24625,12 @@
         <v>4068</v>
       </c>
       <c r="D695" s="4" t="s">
-        <v>4900</v>
+        <v>4898</v>
       </c>
     </row>
     <row r="696" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A696" s="4" t="s">
-        <v>4912</v>
+        <v>4910</v>
       </c>
       <c r="B696" s="4" t="s">
         <v>1934</v>
@@ -24641,7 +24644,7 @@
     </row>
     <row r="697" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A697" s="4" t="s">
-        <v>4915</v>
+        <v>4913</v>
       </c>
       <c r="B697" s="4" t="s">
         <v>1935</v>
@@ -24655,7 +24658,7 @@
     </row>
     <row r="698" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A698" s="4" t="s">
-        <v>4913</v>
+        <v>4911</v>
       </c>
       <c r="B698" s="4" t="s">
         <v>1936</v>
@@ -24669,7 +24672,7 @@
     </row>
     <row r="699" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A699" s="4" t="s">
-        <v>4916</v>
+        <v>4914</v>
       </c>
       <c r="B699" s="4" t="s">
         <v>1937</v>
@@ -24683,7 +24686,7 @@
     </row>
     <row r="700" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A700" s="4" t="s">
-        <v>4917</v>
+        <v>4915</v>
       </c>
       <c r="B700" s="4" t="s">
         <v>1938</v>
@@ -24697,7 +24700,7 @@
     </row>
     <row r="701" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A701" s="4" t="s">
-        <v>4918</v>
+        <v>4916</v>
       </c>
       <c r="B701" s="4" t="s">
         <v>1939</v>
@@ -24711,7 +24714,7 @@
     </row>
     <row r="702" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A702" s="4" t="s">
-        <v>4919</v>
+        <v>4917</v>
       </c>
       <c r="B702" s="4" t="s">
         <v>1940</v>
@@ -24725,7 +24728,7 @@
     </row>
     <row r="703" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A703" s="4" t="s">
-        <v>4920</v>
+        <v>4918</v>
       </c>
       <c r="B703" s="4" t="s">
         <v>1941</v>
@@ -24739,7 +24742,7 @@
     </row>
     <row r="704" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A704" s="4" t="s">
-        <v>4921</v>
+        <v>4919</v>
       </c>
       <c r="B704" s="4" t="s">
         <v>1942</v>
@@ -24753,7 +24756,7 @@
     </row>
     <row r="705" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A705" s="4" t="s">
-        <v>4922</v>
+        <v>4920</v>
       </c>
       <c r="B705" s="4" t="s">
         <v>1048</v>
@@ -24767,7 +24770,7 @@
     </row>
     <row r="706" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A706" s="4" t="s">
-        <v>4914</v>
+        <v>4912</v>
       </c>
       <c r="B706" s="4" t="s">
         <v>1943</v>
@@ -24781,7 +24784,7 @@
     </row>
     <row r="707" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A707" s="4" t="s">
-        <v>4923</v>
+        <v>4921</v>
       </c>
       <c r="B707" s="4" t="s">
         <v>1944</v>
@@ -24795,7 +24798,7 @@
     </row>
     <row r="708" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A708" s="4" t="s">
-        <v>4924</v>
+        <v>4922</v>
       </c>
       <c r="B708" s="4" t="s">
         <v>1945</v>
@@ -24809,7 +24812,7 @@
     </row>
     <row r="709" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A709" s="4" t="s">
-        <v>4925</v>
+        <v>4923</v>
       </c>
       <c r="B709" s="4" t="s">
         <v>1946</v>
@@ -24823,7 +24826,7 @@
     </row>
     <row r="710" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A710" s="4" t="s">
-        <v>4926</v>
+        <v>4924</v>
       </c>
       <c r="B710" s="4" t="s">
         <v>1947</v>
@@ -24837,7 +24840,7 @@
     </row>
     <row r="711" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A711" s="4" t="s">
-        <v>4927</v>
+        <v>4925</v>
       </c>
       <c r="B711" s="4" t="s">
         <v>1948</v>
@@ -24851,7 +24854,7 @@
     </row>
     <row r="712" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A712" s="4" t="s">
-        <v>4928</v>
+        <v>4926</v>
       </c>
       <c r="B712" s="4" t="s">
         <v>1949</v>
@@ -24865,7 +24868,7 @@
     </row>
     <row r="713" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A713" s="4" t="s">
-        <v>4929</v>
+        <v>4927</v>
       </c>
       <c r="B713" s="4" t="s">
         <v>1950</v>
@@ -24879,7 +24882,7 @@
     </row>
     <row r="714" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A714" s="4" t="s">
-        <v>4930</v>
+        <v>4928</v>
       </c>
       <c r="B714" s="4" t="s">
         <v>1951</v>
@@ -24893,7 +24896,7 @@
     </row>
     <row r="715" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A715" s="4" t="s">
-        <v>4931</v>
+        <v>4929</v>
       </c>
       <c r="B715" s="4" t="s">
         <v>1952</v>
@@ -24907,7 +24910,7 @@
     </row>
     <row r="716" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A716" s="4" t="s">
-        <v>4932</v>
+        <v>4930</v>
       </c>
       <c r="B716" s="4" t="s">
         <v>1953</v>
@@ -24921,7 +24924,7 @@
     </row>
     <row r="717" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A717" s="4" t="s">
-        <v>4933</v>
+        <v>4931</v>
       </c>
       <c r="B717" s="4" t="s">
         <v>1954</v>
@@ -24935,7 +24938,7 @@
     </row>
     <row r="718" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A718" s="4" t="s">
-        <v>4934</v>
+        <v>4932</v>
       </c>
       <c r="B718" s="4" t="s">
         <v>1955</v>
@@ -24949,7 +24952,7 @@
     </row>
     <row r="719" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A719" s="4" t="s">
-        <v>4935</v>
+        <v>4933</v>
       </c>
       <c r="B719" s="4" t="s">
         <v>1956</v>
@@ -24963,7 +24966,7 @@
     </row>
     <row r="720" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A720" s="4" t="s">
-        <v>4937</v>
+        <v>4935</v>
       </c>
       <c r="B720" s="4" t="s">
         <v>1957</v>
@@ -24977,7 +24980,7 @@
     </row>
     <row r="721" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A721" s="4" t="s">
-        <v>4938</v>
+        <v>4936</v>
       </c>
       <c r="B721" s="4" t="s">
         <v>1958</v>
@@ -24991,7 +24994,7 @@
     </row>
     <row r="722" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A722" s="4" t="s">
-        <v>4939</v>
+        <v>4937</v>
       </c>
       <c r="B722" s="4" t="s">
         <v>1959</v>
@@ -25005,7 +25008,7 @@
     </row>
     <row r="723" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A723" s="4" t="s">
-        <v>4940</v>
+        <v>4938</v>
       </c>
       <c r="B723" s="4" t="s">
         <v>1960</v>
@@ -25019,7 +25022,7 @@
     </row>
     <row r="724" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A724" s="4" t="s">
-        <v>4936</v>
+        <v>4934</v>
       </c>
       <c r="B724" s="4" t="s">
         <v>1961</v>
@@ -25033,7 +25036,7 @@
     </row>
     <row r="725" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A725" s="4" t="s">
-        <v>4941</v>
+        <v>4939</v>
       </c>
       <c r="B725" s="4" t="s">
         <v>1962</v>
@@ -25047,7 +25050,7 @@
     </row>
     <row r="726" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A726" s="4" t="s">
-        <v>4942</v>
+        <v>4940</v>
       </c>
       <c r="B726" s="4" t="s">
         <v>1963</v>
@@ -25061,7 +25064,7 @@
     </row>
     <row r="727" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A727" s="4" t="s">
-        <v>4944</v>
+        <v>4942</v>
       </c>
       <c r="B727" s="4" t="s">
         <v>1964</v>
@@ -25075,7 +25078,7 @@
     </row>
     <row r="728" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A728" s="4" t="s">
-        <v>4945</v>
+        <v>4943</v>
       </c>
       <c r="B728" s="4" t="s">
         <v>1050</v>
@@ -25089,7 +25092,7 @@
     </row>
     <row r="729" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A729" s="4" t="s">
-        <v>4946</v>
+        <v>4944</v>
       </c>
       <c r="B729" s="4" t="s">
         <v>1965</v>
@@ -25103,7 +25106,7 @@
     </row>
     <row r="730" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A730" s="4" t="s">
-        <v>4943</v>
+        <v>4941</v>
       </c>
       <c r="B730" s="4" t="s">
         <v>1052</v>
@@ -25117,7 +25120,7 @@
     </row>
     <row r="731" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A731" s="4" t="s">
-        <v>4954</v>
+        <v>4952</v>
       </c>
       <c r="B731" s="4" t="s">
         <v>1966</v>
@@ -25131,7 +25134,7 @@
     </row>
     <row r="732" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A732" s="4" t="s">
-        <v>4955</v>
+        <v>4953</v>
       </c>
       <c r="B732" s="4" t="s">
         <v>1967</v>
@@ -25145,7 +25148,7 @@
     </row>
     <row r="733" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A733" s="4" t="s">
-        <v>4952</v>
+        <v>4950</v>
       </c>
       <c r="B733" s="4" t="s">
         <v>1968</v>
@@ -25159,7 +25162,7 @@
     </row>
     <row r="734" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A734" s="4" t="s">
-        <v>4953</v>
+        <v>4951</v>
       </c>
       <c r="B734" s="4" t="s">
         <v>1969</v>
@@ -25173,7 +25176,7 @@
     </row>
     <row r="735" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A735" s="4" t="s">
-        <v>4956</v>
+        <v>4954</v>
       </c>
       <c r="B735" s="4" t="s">
         <v>1970</v>
@@ -25187,7 +25190,7 @@
     </row>
     <row r="736" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A736" s="4" t="s">
-        <v>4957</v>
+        <v>4955</v>
       </c>
       <c r="B736" s="4" t="s">
         <v>1971</v>
@@ -25201,7 +25204,7 @@
     </row>
     <row r="737" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A737" s="4" t="s">
-        <v>4958</v>
+        <v>4956</v>
       </c>
       <c r="B737" s="4" t="s">
         <v>1972</v>
@@ -25215,7 +25218,7 @@
     </row>
     <row r="738" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A738" s="4" t="s">
-        <v>4959</v>
+        <v>4957</v>
       </c>
       <c r="B738" s="4" t="s">
         <v>1973</v>
@@ -25229,7 +25232,7 @@
     </row>
     <row r="739" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A739" s="4" t="s">
-        <v>4960</v>
+        <v>4958</v>
       </c>
       <c r="B739" s="4" t="s">
         <v>1974</v>
@@ -25243,7 +25246,7 @@
     </row>
     <row r="740" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A740" s="4" t="s">
-        <v>4961</v>
+        <v>4959</v>
       </c>
       <c r="B740" s="4" t="s">
         <v>1975</v>
@@ -25257,7 +25260,7 @@
     </row>
     <row r="741" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A741" s="4" t="s">
-        <v>4962</v>
+        <v>4960</v>
       </c>
       <c r="B741" s="4" t="s">
         <v>1976</v>
@@ -25271,7 +25274,7 @@
     </row>
     <row r="742" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A742" s="4" t="s">
-        <v>4963</v>
+        <v>4961</v>
       </c>
       <c r="B742" s="4" t="s">
         <v>1977</v>
@@ -25285,7 +25288,7 @@
     </row>
     <row r="743" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A743" s="4" t="s">
-        <v>4964</v>
+        <v>4962</v>
       </c>
       <c r="B743" s="4" t="s">
         <v>1978</v>
@@ -25299,7 +25302,7 @@
     </row>
     <row r="744" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A744" s="4" t="s">
-        <v>4965</v>
+        <v>4963</v>
       </c>
       <c r="B744" s="4" t="s">
         <v>1979</v>
@@ -25313,7 +25316,7 @@
     </row>
     <row r="745" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A745" s="4" t="s">
-        <v>4966</v>
+        <v>4964</v>
       </c>
       <c r="B745" s="4" t="s">
         <v>1980</v>
@@ -25327,7 +25330,7 @@
     </row>
     <row r="746" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A746" s="4" t="s">
-        <v>4967</v>
+        <v>4965</v>
       </c>
       <c r="B746" s="4" t="s">
         <v>1981</v>
@@ -25341,7 +25344,7 @@
     </row>
     <row r="747" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A747" s="4" t="s">
-        <v>4968</v>
+        <v>4966</v>
       </c>
       <c r="B747" s="4" t="s">
         <v>1982</v>
@@ -25355,7 +25358,7 @@
     </row>
     <row r="748" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A748" s="4" t="s">
-        <v>4969</v>
+        <v>4967</v>
       </c>
       <c r="B748" s="4" t="s">
         <v>1983</v>
@@ -25369,7 +25372,7 @@
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A749" s="4" t="s">
-        <v>4970</v>
+        <v>4968</v>
       </c>
       <c r="B749" s="4" t="s">
         <v>1984</v>
@@ -25383,7 +25386,7 @@
     </row>
     <row r="750" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A750" s="4" t="s">
-        <v>4971</v>
+        <v>4969</v>
       </c>
       <c r="B750" s="4" t="s">
         <v>1985</v>
@@ -25397,7 +25400,7 @@
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A751" s="4" t="s">
-        <v>4972</v>
+        <v>4970</v>
       </c>
       <c r="B751" s="4" t="s">
         <v>1986</v>
@@ -25411,7 +25414,7 @@
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A752" s="4" t="s">
-        <v>4973</v>
+        <v>4971</v>
       </c>
       <c r="B752" s="4" t="s">
         <v>1056</v>
@@ -25425,7 +25428,7 @@
     </row>
     <row r="753" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A753" s="4" t="s">
-        <v>4974</v>
+        <v>4972</v>
       </c>
       <c r="B753" s="4" t="s">
         <v>1987</v>
@@ -25439,7 +25442,7 @@
     </row>
     <row r="754" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A754" s="4" t="s">
-        <v>4975</v>
+        <v>4973</v>
       </c>
       <c r="B754" s="4" t="s">
         <v>1988</v>
@@ -25453,7 +25456,7 @@
     </row>
     <row r="755" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A755" s="4" t="s">
-        <v>4976</v>
+        <v>4974</v>
       </c>
       <c r="B755" s="4" t="s">
         <v>1058</v>
@@ -25467,7 +25470,7 @@
     </row>
     <row r="756" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A756" s="4" t="s">
-        <v>4977</v>
+        <v>4975</v>
       </c>
       <c r="B756" s="4" t="s">
         <v>1989</v>
@@ -25481,7 +25484,7 @@
     </row>
     <row r="757" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A757" s="4" t="s">
-        <v>4978</v>
+        <v>4976</v>
       </c>
       <c r="B757" s="4" t="s">
         <v>1990</v>
@@ -25495,7 +25498,7 @@
     </row>
     <row r="758" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A758" s="4" t="s">
-        <v>4979</v>
+        <v>4977</v>
       </c>
       <c r="B758" s="4" t="s">
         <v>1991</v>
@@ -25509,7 +25512,7 @@
     </row>
     <row r="759" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A759" s="4" t="s">
-        <v>4980</v>
+        <v>4978</v>
       </c>
       <c r="B759" s="4" t="s">
         <v>1992</v>
@@ -25706,7 +25709,7 @@
     </row>
     <row r="778" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A778" s="4" t="s">
-        <v>4950</v>
+        <v>4948</v>
       </c>
       <c r="B778" s="4" t="s">
         <v>2948</v>
@@ -25715,7 +25718,7 @@
         <v>4146</v>
       </c>
       <c r="D778" s="4" t="s">
-        <v>4951</v>
+        <v>4949</v>
       </c>
     </row>
     <row r="779" spans="1:4" x14ac:dyDescent="0.25">
@@ -25759,12 +25762,12 @@
         <v>4149</v>
       </c>
       <c r="D782" s="4" t="s">
-        <v>4947</v>
+        <v>4945</v>
       </c>
     </row>
     <row r="783" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A783" s="4" t="s">
-        <v>4949</v>
+        <v>4947</v>
       </c>
       <c r="B783" s="4" t="s">
         <v>2955</v>
@@ -25773,7 +25776,7 @@
         <v>4150</v>
       </c>
       <c r="D783" s="4" t="s">
-        <v>4948</v>
+        <v>4946</v>
       </c>
     </row>
     <row r="784" spans="1:4" x14ac:dyDescent="0.25">
@@ -26480,7 +26483,7 @@
     </row>
     <row r="847" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A847" s="4" t="s">
-        <v>4674</v>
+        <v>4672</v>
       </c>
       <c r="B847" s="4" t="s">
         <v>659</v>
@@ -26699,7 +26702,7 @@
     </row>
     <row r="865" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A865" s="4" t="s">
-        <v>4676</v>
+        <v>4674</v>
       </c>
       <c r="B865" s="4" t="s">
         <v>720</v>
@@ -31053,7 +31056,7 @@
     </row>
     <row r="1260" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1260" s="4" t="s">
-        <v>4675</v>
+        <v>4673</v>
       </c>
       <c r="B1260" s="4" t="s">
         <v>641</v>
@@ -31243,7 +31246,7 @@
     </row>
     <row r="1277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1277" s="4" t="s">
-        <v>4677</v>
+        <v>4675</v>
       </c>
       <c r="B1277" s="4" t="s">
         <v>2541</v>
@@ -31271,7 +31274,7 @@
     </row>
     <row r="1279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1279" s="4" t="s">
-        <v>4679</v>
+        <v>4677</v>
       </c>
       <c r="B1279" s="4" t="s">
         <v>900</v>
@@ -31285,7 +31288,7 @@
     </row>
     <row r="1280" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1280" s="4" t="s">
-        <v>4678</v>
+        <v>4676</v>
       </c>
       <c r="B1280" s="4" t="s">
         <v>784</v>

</xml_diff>